<commit_message>
update files from 4 to 9 + metadata
</commit_message>
<xml_diff>
--- a/metadata_project.xlsx
+++ b/metadata_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ludivine/Desktop/TERMSUITE_WORKSPACE/terminology_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751BF5AC-ED57-364A-B4AD-4562B18A158E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB093322-5E60-F14C-8C56-F2CB1085ABC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{7FEF5D0A-BA71-684F-80B1-5965CE06493C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>number</t>
   </si>
@@ -43,75 +43,18 @@
     <t>article title</t>
   </si>
   <si>
-    <t>TUNDRA: A Multilingual Corpus of Found Data for TTS Research Created</t>
-  </si>
-  <si>
     <t>Current trends in multilingual speech processing</t>
   </si>
   <si>
-    <t>Learning to Speak Fluently in a Foreign Language:</t>
-  </si>
-  <si>
-    <t>One Model, Many Languages: Meta-learning for Multilingual Text-to-Speech</t>
-  </si>
-  <si>
-    <t>DIRECTLY MODELING SPEECHWAVEFORMS BY NEURAL NETWORKS</t>
-  </si>
-  <si>
-    <t>FOR STATISTICAL PARAMETRIC SPEECH SYNTHESIS</t>
-  </si>
-  <si>
-    <t>Multilingual Text Analysis for Text-to-Speech Synthesis</t>
-  </si>
-  <si>
-    <t>TEXT-TO-SPEECH CONVERSION WITH NEURAL NETWORKS:</t>
-  </si>
-  <si>
-    <t>Merlin: An Open Source Neural Network Speech Synthesis System</t>
-  </si>
-  <si>
-    <t>Grapheme-to-Phoneme Conversion with</t>
-  </si>
-  <si>
-    <t>GlobalPhone: A Multilingual Text &amp; Speech Database in 20 Languages</t>
-  </si>
-  <si>
-    <t>MULTILINGUAL TEXT-TO-SPEECH SYNTHESIS</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>MELLOTRON: MULTISPEAKER EXPRESSIVE VOICE SYNTHESIS BY CONDITIONING</t>
-  </si>
-  <si>
     <t>Text Preprocessing for Speech Synthesis</t>
   </si>
   <si>
     <t>Unsupervised and lightly-supervised learning for rapid construction of TTS</t>
   </si>
   <si>
-    <t>STATISTICAL PARAMETRIC SPEECH SYNTHESIS</t>
-  </si>
-  <si>
-    <r>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ACOTRON: TOWARDS END-TO-END SPEECH SYNTHESIS</t>
-    </r>
-  </si>
-  <si>
-    <t>Non-Autoregressive Neural Text-to-Speech</t>
-  </si>
-  <si>
     <t>run tagger (with IOB tagset)</t>
   </si>
   <si>
@@ -134,6 +77,48 @@
   </si>
   <si>
     <t>don't need</t>
+  </si>
+  <si>
+    <t>Directly modeling speech waveforms by neural networks</t>
+  </si>
+  <si>
+    <t>Text-to-Speech conveersion with neurzl networks</t>
+  </si>
+  <si>
+    <t>Multilingual Text-to-Speech synthesis</t>
+  </si>
+  <si>
+    <t>MELLOTRON: Multispeaker expressive voice synthesis by conditioning</t>
+  </si>
+  <si>
+    <t>Statistical parametric speech synthesis</t>
+  </si>
+  <si>
+    <t>TACOTRON: Toward end-to-end speech synthesis</t>
+  </si>
+  <si>
+    <t>TUNDRA: A multilingual corpus of found data for TTS research created</t>
+  </si>
+  <si>
+    <t>Learning to speak fluently in a foreign language:</t>
+  </si>
+  <si>
+    <t>One model, many languages: meta-learning for multilingual Text-to-Speech</t>
+  </si>
+  <si>
+    <t>Non-autoregressive neural Text-to-Speech</t>
+  </si>
+  <si>
+    <t>Multilingual text Aanalysis for Text-to-Speech synthesis</t>
+  </si>
+  <si>
+    <t>Grapheme-to-Phoneme conversion with convoltional neural networks</t>
+  </si>
+  <si>
+    <t>GlobalPhone: A multilingual Text &amp; Speech database in 20 Languages</t>
+  </si>
+  <si>
+    <t>MERLIN: An open source neural network speech synthesis system</t>
   </si>
 </sst>
 </file>
@@ -497,7 +482,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -522,10 +507,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -533,10 +518,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -544,10 +529,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -555,7 +540,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -563,7 +551,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -571,23 +562,27 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -595,7 +590,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -603,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -611,7 +609,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -631,7 +629,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -639,7 +637,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -647,7 +645,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -655,7 +653,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -663,7 +661,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -671,7 +669,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -679,7 +677,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -698,7 +696,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -727,7 +725,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -735,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -743,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -751,7 +749,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout 3 articles en txt
</commit_message>
<xml_diff>
--- a/metadata_project.xlsx
+++ b/metadata_project.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t xml:space="preserve">number</t>
   </si>
@@ -56,6 +56,9 @@
     <t xml:space="preserve">Directly modeling speech waveforms by neural networks</t>
   </si>
   <si>
+    <t xml:space="preserve">Transfer Learning from Speaker Verification to Multispeaker Text-To-Speech Synthesis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multilingual text Aanalysis for Text-to-Speech synthesis</t>
   </si>
   <si>
@@ -68,10 +71,16 @@
     <t xml:space="preserve">Grapheme-to-Phoneme conversion with convoltional neural networks</t>
   </si>
   <si>
+    <t xml:space="preserve">FastSpeech: Fast, Robust and Controllable Text to Speech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep Voice: Real-time Neural Text-to-Speech</t>
+  </si>
+  <si>
     <t xml:space="preserve">GlobalPhone: A multilingual Text &amp; Speech database in 20 Languages</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">Deep Voice 2: Multi-Speaker Neural Text-to-Speech</t>
   </si>
   <si>
     <t xml:space="preserve">Multilingual Text-to-Speech synthesis</t>
@@ -187,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -198,6 +207,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -280,13 +293,13 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="86.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="86.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.61"/>
   </cols>
@@ -368,18 +381,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>4</v>
@@ -390,7 +405,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>4</v>
@@ -401,7 +416,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>4</v>
@@ -412,30 +427,40 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>4</v>
@@ -452,12 +477,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,7 +493,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>4</v>
@@ -476,7 +504,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,7 +515,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,7 +523,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,7 +531,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,7 +539,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -545,7 +576,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,7 +608,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>